<commit_message>
update 29-10-16, see the original github page for the changes
</commit_message>
<xml_diff>
--- a/werkverdeling/aantal werkuren.xlsx
+++ b/werkverdeling/aantal werkuren.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Logboek Totalen" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>INFORMATICA</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>grote update planner</t>
+  </si>
+  <si>
+    <t>leren html 5 en maken oefen project (renesteeman.net/time)</t>
+  </si>
+  <si>
+    <t>leren css3 en toevoegen speciale styling voor form posts met css3 (grotere eerste letter post en afwisselende background-color posts</t>
   </si>
 </sst>
 </file>
@@ -213,9 +219,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -378,41 +391,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -428,7 +444,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -737,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -768,11 +784,11 @@
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -794,11 +810,11 @@
       </c>
       <c r="C5">
         <f>tot_teamlid1</f>
-        <v>3440</v>
+        <v>3560</v>
       </c>
       <c r="D5" s="4">
         <f>C5/60</f>
-        <v>57.333333333333336</v>
+        <v>59.333333333333336</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,7 +839,7 @@
       </c>
       <c r="D8" s="5">
         <f>SUM(D5:D6)</f>
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -857,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1205,7 @@
       <c r="B29" s="18">
         <v>42667</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>50</v>
       </c>
       <c r="D29">
@@ -1200,10 +1216,32 @@
       <c r="B30" s="18">
         <v>42667</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>51</v>
       </c>
       <c r="D30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="18">
+        <v>42668</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="18">
+        <v>42672</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32">
         <v>60</v>
       </c>
     </row>
@@ -1213,7 +1251,7 @@
       </c>
       <c r="D43">
         <f>SUM(D3:D42)</f>
-        <v>3440</v>
+        <v>3560</v>
       </c>
     </row>
   </sheetData>
@@ -1360,21 +1398,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D49BEEDDDF0DF64CBE3D65DA0999E19A" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="ae4efb83b009937fa6d8406911710d81">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c01a820-ee70-4c37-af38-f30911af0ad8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ebabd3000020209bf13b285d48368bf4" ns2:_="">
     <xsd:import namespace="9c01a820-ee70-4c37-af38-f30911af0ad8"/>
@@ -1522,10 +1545,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D2D534C-462C-4F23-9AD5-3681B055117A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FB08530-EBDB-470A-A832-4BE30F9AA86F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c01a820-ee70-4c37-af38-f30911af0ad8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1547,19 +1595,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FB08530-EBDB-470A-A832-4BE30F9AA86F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D2D534C-462C-4F23-9AD5-3681B055117A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9c01a820-ee70-4c37-af38-f30911af0ad8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update 31-10, check old github page for more info
</commit_message>
<xml_diff>
--- a/werkverdeling/aantal werkuren.xlsx
+++ b/werkverdeling/aantal werkuren.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Logboek Totalen" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,7 @@
     <t>leren html 5 en maken oefen project (renesteeman.net/time)</t>
   </si>
   <si>
-    <t>leren css3 en toevoegen speciale styling voor form posts met css3 (grotere eerste letter post en afwisselende background-color posts</t>
+    <t>leren css3 en toevoegen speciale styling voor form posts met css3 (grotere eerste letter post, afwisselende background-color posts, animatie bij hover posts en text-shadow)</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -810,11 +810,11 @@
       </c>
       <c r="C5">
         <f>tot_teamlid1</f>
-        <v>3560</v>
+        <v>3590</v>
       </c>
       <c r="D5" s="4">
         <f>C5/60</f>
-        <v>59.333333333333336</v>
+        <v>59.833333333333336</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
       </c>
       <c r="D8" s="5">
         <f>SUM(D5:D6)</f>
-        <v>88</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1242,7 @@
         <v>53</v>
       </c>
       <c r="D32">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D43">
         <f>SUM(D3:D42)</f>
-        <v>3560</v>
+        <v>3590</v>
       </c>
     </row>
   </sheetData>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>